<commit_message>
Updated ZAF model - 2025-08-01 01:41
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_336.xlsx
+++ b/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_336.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2530A199-6B6E-4F9A-A2C4-F9E321848F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897CBFD0-E7C0-474B-8E00-72710D9AD21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5011" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5080" uniqueCount="518">
   <si>
     <t>UC_N</t>
   </si>
@@ -1569,10 +1569,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16</t>
-  </si>
-  <si>
-    <t>m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m07ah03,m07ah21,m10ah03,m12ah05,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01</t>
+    <t>m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15</t>
+  </si>
+  <si>
+    <t>m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m07ah03,m07ah21,m10ah03,m12ah05,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m07ah03,m07ah21,m10ah03,m12ah05,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01</v>
+        <v>m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m07ah03,m07ah21,m10ah03,m12ah05,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16</v>
+        <v>m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2788,7 +2788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF22551-73F3-4993-AC68-FD8030EB4814}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B401446D-3BEC-4A29-8153-5548E2976C40}">
   <dimension ref="B2:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2875,6 +2875,9 @@
       <c r="D7" t="s">
         <v>86</v>
       </c>
+      <c r="E7" t="s">
+        <v>79</v>
+      </c>
       <c r="F7" t="s">
         <v>62</v>
       </c>
@@ -2886,6 +2889,9 @@
       <c r="D8" t="s">
         <v>88</v>
       </c>
+      <c r="E8" t="s">
+        <v>79</v>
+      </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
@@ -2897,6 +2903,9 @@
       <c r="D9" t="s">
         <v>90</v>
       </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
       <c r="F9" t="s">
         <v>62</v>
       </c>
@@ -2908,6 +2917,9 @@
       <c r="D10" t="s">
         <v>91</v>
       </c>
+      <c r="E10" t="s">
+        <v>79</v>
+      </c>
       <c r="F10" t="s">
         <v>62</v>
       </c>
@@ -2919,6 +2931,9 @@
       <c r="D11" t="s">
         <v>93</v>
       </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
       <c r="F11" t="s">
         <v>62</v>
       </c>
@@ -2930,6 +2945,9 @@
       <c r="D12" t="s">
         <v>95</v>
       </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
       <c r="F12" t="s">
         <v>62</v>
       </c>
@@ -2941,6 +2959,9 @@
       <c r="D13" t="s">
         <v>97</v>
       </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
       <c r="F13" t="s">
         <v>62</v>
       </c>
@@ -2952,6 +2973,9 @@
       <c r="D14" t="s">
         <v>99</v>
       </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
       <c r="F14" t="s">
         <v>62</v>
       </c>
@@ -2963,6 +2987,9 @@
       <c r="D15" t="s">
         <v>101</v>
       </c>
+      <c r="E15" t="s">
+        <v>79</v>
+      </c>
       <c r="F15" t="s">
         <v>62</v>
       </c>
@@ -2971,6 +2998,9 @@
       <c r="D16" t="s">
         <v>102</v>
       </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
       <c r="F16" t="s">
         <v>62</v>
       </c>
@@ -2979,6 +3009,9 @@
       <c r="D17" t="s">
         <v>103</v>
       </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
       <c r="F17" t="s">
         <v>62</v>
       </c>
@@ -2987,6 +3020,9 @@
       <c r="D18" t="s">
         <v>104</v>
       </c>
+      <c r="E18" t="s">
+        <v>79</v>
+      </c>
       <c r="F18" t="s">
         <v>62</v>
       </c>
@@ -2995,6 +3031,9 @@
       <c r="D19" t="s">
         <v>105</v>
       </c>
+      <c r="E19" t="s">
+        <v>79</v>
+      </c>
       <c r="F19" t="s">
         <v>62</v>
       </c>
@@ -3003,6 +3042,9 @@
       <c r="D20" t="s">
         <v>106</v>
       </c>
+      <c r="E20" t="s">
+        <v>79</v>
+      </c>
       <c r="F20" t="s">
         <v>62</v>
       </c>
@@ -3011,6 +3053,9 @@
       <c r="D21" t="s">
         <v>107</v>
       </c>
+      <c r="E21" t="s">
+        <v>79</v>
+      </c>
       <c r="F21" t="s">
         <v>62</v>
       </c>
@@ -3019,6 +3064,9 @@
       <c r="D22" t="s">
         <v>108</v>
       </c>
+      <c r="E22" t="s">
+        <v>79</v>
+      </c>
       <c r="F22" t="s">
         <v>62</v>
       </c>
@@ -3027,6 +3075,9 @@
       <c r="D23" t="s">
         <v>109</v>
       </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
       <c r="F23" t="s">
         <v>62</v>
       </c>
@@ -3035,6 +3086,9 @@
       <c r="D24" t="s">
         <v>110</v>
       </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
       <c r="F24" t="s">
         <v>62</v>
       </c>
@@ -3043,6 +3097,9 @@
       <c r="D25" t="s">
         <v>111</v>
       </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
       <c r="F25" t="s">
         <v>62</v>
       </c>
@@ -3051,6 +3108,9 @@
       <c r="D26" t="s">
         <v>112</v>
       </c>
+      <c r="E26" t="s">
+        <v>79</v>
+      </c>
       <c r="F26" t="s">
         <v>62</v>
       </c>
@@ -3059,6 +3119,9 @@
       <c r="D27" t="s">
         <v>113</v>
       </c>
+      <c r="E27" t="s">
+        <v>79</v>
+      </c>
       <c r="F27" t="s">
         <v>62</v>
       </c>
@@ -3067,384 +3130,528 @@
       <c r="D28" t="s">
         <v>114</v>
       </c>
+      <c r="E28" t="s">
+        <v>79</v>
+      </c>
       <c r="F28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D29" t="s">
         <v>115</v>
       </c>
+      <c r="E29" t="s">
+        <v>79</v>
+      </c>
       <c r="F29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D30" t="s">
         <v>116</v>
       </c>
+      <c r="E30" t="s">
+        <v>79</v>
+      </c>
       <c r="F30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D31" t="s">
         <v>117</v>
       </c>
+      <c r="E31" t="s">
+        <v>79</v>
+      </c>
       <c r="F31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D32" t="s">
         <v>118</v>
       </c>
+      <c r="E32" t="s">
+        <v>79</v>
+      </c>
       <c r="F32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D33" t="s">
         <v>119</v>
       </c>
+      <c r="E33" t="s">
+        <v>79</v>
+      </c>
       <c r="F33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D34" t="s">
         <v>120</v>
       </c>
+      <c r="E34" t="s">
+        <v>79</v>
+      </c>
       <c r="F34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D35" t="s">
         <v>121</v>
       </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
       <c r="F35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D36" t="s">
         <v>122</v>
       </c>
+      <c r="E36" t="s">
+        <v>79</v>
+      </c>
       <c r="F36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D37" t="s">
         <v>123</v>
       </c>
+      <c r="E37" t="s">
+        <v>79</v>
+      </c>
       <c r="F37" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D38" t="s">
         <v>124</v>
       </c>
+      <c r="E38" t="s">
+        <v>79</v>
+      </c>
       <c r="F38" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D39" t="s">
         <v>125</v>
       </c>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
       <c r="F39" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D40" t="s">
         <v>126</v>
       </c>
+      <c r="E40" t="s">
+        <v>79</v>
+      </c>
       <c r="F40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D41" t="s">
         <v>127</v>
       </c>
+      <c r="E41" t="s">
+        <v>79</v>
+      </c>
       <c r="F41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D42" t="s">
         <v>128</v>
       </c>
+      <c r="E42" t="s">
+        <v>79</v>
+      </c>
       <c r="F42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D43" t="s">
         <v>129</v>
       </c>
+      <c r="E43" t="s">
+        <v>79</v>
+      </c>
       <c r="F43" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D44" t="s">
         <v>130</v>
       </c>
+      <c r="E44" t="s">
+        <v>79</v>
+      </c>
       <c r="F44" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D45" t="s">
         <v>131</v>
       </c>
+      <c r="E45" t="s">
+        <v>79</v>
+      </c>
       <c r="F45" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D46" t="s">
         <v>132</v>
       </c>
+      <c r="E46" t="s">
+        <v>79</v>
+      </c>
       <c r="F46" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D47" t="s">
         <v>133</v>
       </c>
+      <c r="E47" t="s">
+        <v>79</v>
+      </c>
       <c r="F47" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
         <v>134</v>
       </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
       <c r="F48" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
         <v>135</v>
       </c>
+      <c r="E49" t="s">
+        <v>79</v>
+      </c>
       <c r="F49" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
         <v>136</v>
       </c>
+      <c r="E50" t="s">
+        <v>79</v>
+      </c>
       <c r="F50" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
         <v>137</v>
       </c>
+      <c r="E51" t="s">
+        <v>79</v>
+      </c>
       <c r="F51" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
         <v>138</v>
       </c>
+      <c r="E52" t="s">
+        <v>79</v>
+      </c>
       <c r="F52" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
         <v>139</v>
       </c>
+      <c r="E53" t="s">
+        <v>79</v>
+      </c>
       <c r="F53" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D54" t="s">
         <v>140</v>
       </c>
+      <c r="E54" t="s">
+        <v>79</v>
+      </c>
       <c r="F54" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D55" t="s">
         <v>141</v>
       </c>
+      <c r="E55" t="s">
+        <v>79</v>
+      </c>
       <c r="F55" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D56" t="s">
         <v>142</v>
       </c>
+      <c r="E56" t="s">
+        <v>79</v>
+      </c>
       <c r="F56" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D57" t="s">
         <v>143</v>
       </c>
+      <c r="E57" t="s">
+        <v>79</v>
+      </c>
       <c r="F57" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D58" t="s">
         <v>144</v>
       </c>
+      <c r="E58" t="s">
+        <v>79</v>
+      </c>
       <c r="F58" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D59" t="s">
         <v>145</v>
       </c>
+      <c r="E59" t="s">
+        <v>79</v>
+      </c>
       <c r="F59" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D60" t="s">
         <v>146</v>
       </c>
+      <c r="E60" t="s">
+        <v>79</v>
+      </c>
       <c r="F60" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D61" t="s">
         <v>147</v>
       </c>
+      <c r="E61" t="s">
+        <v>79</v>
+      </c>
       <c r="F61" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D62" t="s">
         <v>148</v>
       </c>
+      <c r="E62" t="s">
+        <v>79</v>
+      </c>
       <c r="F62" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D63" t="s">
         <v>149</v>
       </c>
+      <c r="E63" t="s">
+        <v>79</v>
+      </c>
       <c r="F63" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D64" t="s">
         <v>150</v>
       </c>
+      <c r="E64" t="s">
+        <v>79</v>
+      </c>
       <c r="F64" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D65" t="s">
         <v>151</v>
       </c>
+      <c r="E65" t="s">
+        <v>79</v>
+      </c>
       <c r="F65" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D66" t="s">
         <v>152</v>
       </c>
+      <c r="E66" t="s">
+        <v>79</v>
+      </c>
       <c r="F66" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D67" t="s">
         <v>153</v>
       </c>
+      <c r="E67" t="s">
+        <v>79</v>
+      </c>
       <c r="F67" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D68" t="s">
         <v>154</v>
       </c>
+      <c r="E68" t="s">
+        <v>79</v>
+      </c>
       <c r="F68" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D69" t="s">
         <v>155</v>
       </c>
+      <c r="E69" t="s">
+        <v>79</v>
+      </c>
       <c r="F69" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D70" t="s">
         <v>156</v>
       </c>
+      <c r="E70" t="s">
+        <v>79</v>
+      </c>
       <c r="F70" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D71" t="s">
         <v>157</v>
       </c>
+      <c r="E71" t="s">
+        <v>79</v>
+      </c>
       <c r="F71" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D72" t="s">
         <v>158</v>
       </c>
+      <c r="E72" t="s">
+        <v>79</v>
+      </c>
       <c r="F72" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D73" t="s">
         <v>159</v>
       </c>
+      <c r="E73" t="s">
+        <v>79</v>
+      </c>
       <c r="F73" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D74" t="s">
         <v>160</v>
       </c>
+      <c r="E74" t="s">
+        <v>79</v>
+      </c>
       <c r="F74" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D75" t="s">
         <v>161</v>
       </c>
+      <c r="E75" t="s">
+        <v>79</v>
+      </c>
       <c r="F75" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3453,7 +3660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841B3CCB-23F7-471E-95D1-6D4458383D32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2159FD45-D9B9-4863-A934-13ED648E343B}">
   <dimension ref="B2:O339"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3532,10 +3739,10 @@
         <v>168</v>
       </c>
       <c r="M4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="N4">
-        <v>5.8624127617148546E-2</v>
+        <v>4.4267198404785643E-2</v>
       </c>
       <c r="O4" t="s">
         <v>516</v>
@@ -3567,10 +3774,10 @@
         <v>168</v>
       </c>
       <c r="M5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N5">
-        <v>4.4267198404785636E-2</v>
+        <v>4.4267198404785643E-2</v>
       </c>
       <c r="O5" t="s">
         <v>516</v>
@@ -3602,10 +3809,10 @@
         <v>168</v>
       </c>
       <c r="M6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N6">
-        <v>9.2123629112661989E-2</v>
+        <v>4.5463609172482565E-2</v>
       </c>
       <c r="O6" t="s">
         <v>516</v>
@@ -3637,10 +3844,10 @@
         <v>168</v>
       </c>
       <c r="M7" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="N7">
-        <v>0.14715852442671984</v>
+        <v>0.12203389830508475</v>
       </c>
       <c r="O7" t="s">
         <v>516</v>
@@ -3672,10 +3879,10 @@
         <v>168</v>
       </c>
       <c r="M8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="N8">
-        <v>4.5463609172482558E-2</v>
+        <v>5.8624127617148553E-2</v>
       </c>
       <c r="O8" t="s">
         <v>516</v>
@@ -3707,10 +3914,10 @@
         <v>168</v>
       </c>
       <c r="M9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="N9">
-        <v>0.15433698903290127</v>
+        <v>0.1986041874376869</v>
       </c>
       <c r="O9" t="s">
         <v>516</v>
@@ -3742,10 +3949,10 @@
         <v>168</v>
       </c>
       <c r="M10" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="N10">
-        <v>0.16510468594217348</v>
+        <v>0.1543369890329013</v>
       </c>
       <c r="O10" t="s">
         <v>516</v>
@@ -3777,10 +3984,10 @@
         <v>168</v>
       </c>
       <c r="M11" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="N11">
-        <v>7.7766699900299094E-2</v>
+        <v>0.16510468594217348</v>
       </c>
       <c r="O11" t="s">
         <v>516</v>
@@ -3815,7 +4022,7 @@
         <v>96</v>
       </c>
       <c r="N12">
-        <v>5.0249252243270183E-2</v>
+        <v>5.0249252243270197E-2</v>
       </c>
       <c r="O12" t="s">
         <v>516</v>
@@ -3847,10 +4054,10 @@
         <v>168</v>
       </c>
       <c r="M13" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="N13">
-        <v>0.19860418743768687</v>
+        <v>7.7766699900299094E-2</v>
       </c>
       <c r="O13" t="s">
         <v>516</v>
@@ -3882,10 +4089,10 @@
         <v>168</v>
       </c>
       <c r="M14" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="N14">
-        <v>4.4267198404785636E-2</v>
+        <v>9.2123629112662017E-2</v>
       </c>
       <c r="O14" t="s">
         <v>516</v>
@@ -3917,10 +4124,10 @@
         <v>168</v>
       </c>
       <c r="M15" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="N15">
-        <v>0.12203389830508474</v>
+        <v>0.14715852442671987</v>
       </c>
       <c r="O15" t="s">
         <v>516</v>
@@ -12356,7 +12563,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B660891C-6905-4093-AF26-965A65C3EE1F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE042B97-0457-4FD0-9B12-94135A37A91A}">
   <dimension ref="B2:O647"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ZAF model - 2025-08-01 01:53
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_336.xlsx
+++ b/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_336.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897CBFD0-E7C0-474B-8E00-72710D9AD21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706DD819-1D6C-4E39-BE1C-91A5431904A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5080" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5011" uniqueCount="518">
   <si>
     <t>UC_N</t>
   </si>
@@ -1569,10 +1569,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15</t>
-  </si>
-  <si>
-    <t>m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m07ah03,m07ah21,m10ah03,m12ah05,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04</t>
+    <t>m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08</t>
+  </si>
+  <si>
+    <t>m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m07ah03,m07ah21,m10ah03,m12ah05,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m07ah03,m07ah21,m10ah03,m12ah05,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04</v>
+        <v>m02ah02,m02ah19,m02ah21,m03ah20,m07ah19,m07ah23,m07c0716h20,m08ah19,m08ah22,m09ah06,m10ah20,m11ah06,m11ah21,m02ah03,m02ah04,m02ah22,m07ah01,m07ah20,m07c0716h01,m09ah22,m09ah24,m10ah21,m11ah02,m12ah20,m12ah23,m01ah06,m01b0121h01,m02ah06,m03ah03,m04ah06,m05ah03,m05ah20,m06ah01,m06ah23,m07ah22,m09ah21,m12ah04,m01ah02,m01ah19,m01ah22,m01b0121h23,m02ah05,m03ah01,m04ah23,m05ah04,m08ah04,m09ah01,m12ah06,m12ah19,m01ah23,m03ah02,m03ah24,m06ah24,m07ah05,m09ah03,m11ah22,m12ah24,m01ah04,m03ah04,m04ah20,m06ah05,m09ah19,m01b0121h02,m01b0121h05,m01b0121h20,m06ah03,m07ah04,m07c0716h19,m08ah02,m08ah03,m08ah21,m09ah05,m11ah05,m12ah21,m07ah03,m07ah21,m10ah03,m12ah05,m01ah01,m01ah05,m02ah23,m04ah01,m04ah04,m06ah02,m07ah06,m07c0716h02,m07c0716h23,m09ah02,m09ah04,m10ah05,m10ah23,m11ah20,m11ah23,m01b0121h22,m03ah22,m04ah05,m06ah04,m06ah19,m06ah20,m07c0716h04,m07c0716h24,m09ah20,m11ah19,m12ah22,m01b0121h04,m01b0121h06,m01b0121h21,m03ah06,m03ah21,m04ah02,m05ah01,m05ah06,m07c0716h06,m10ah06,m10ah19,m12ah01,m01b0121h03,m02ah20,m03ah23,m04ah22,m07c0716h22,m08ah01,m08ah23,m10ah02,m11ah01,m11ah04,m01ah24,m05ah05,m05ah22,m06ah06,m06ah22,m08ah05,m08ah06,m08ah20,m10ah01,m12ah02,m02ah01,m02ah24,m03ah19,m05ah02,m05ah19,m06ah21,m07c0716h05,m08ah24,m12ah03,m01ah20,m03ah05,m04ah03,m04ah19,m04ah21,m05ah23,m07ah24,m07c0716h03,m07c0716h21,m11ah24,m01ah03,m01ah21,m01b0121h19,m01b0121h24,m04ah24,m05ah21,m05ah24,m07ah02,m09ah23,m10ah04,m10ah22,m10ah24,m11ah03</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15</v>
+        <v>m03ah16,m04ah18,m05ah10,m07ah17,m07c0716h09,m12ah07,m01ah15,m01ah18,m01b0121h14,m02ah07,m04ah08,m04ah14,m05ah07,m05ah13,m07c0716h07,m07c0716h15,m08ah18,m10ah18,m12ah11,m01ah07,m02ah11,m05ah09,m05ah15,m07ah12,m09ah10,m11ah11,m11ah18,m12ah14,m01ah14,m01b0121h15,m01b0121h17,m02ah09,m02ah10,m02ah12,m03ah08,m03ah09,m05ah14,m07c0716h16,m11ah08,m11ah15,m12ah17,m01b0121h08,m02ah15,m04ah17,m07ah09,m07c0716h17,m10ah12,m10ah14,m11ah09,m11ah13,m01ah12,m01ah13,m01b0121h18,m04ah10,m04ah16,m05ah08,m06ah13,m07ah13,m09ah12,m10ah10,m10ah11,m11ah07,m01ah09,m01b0121h09,m01b0121h16,m02ah18,m03ah18,m05ah12,m05ah18,m07c0716h18,m08ah07,m10ah15,m11ah12,m12ah18,m01ah11,m01b0121h10,m03ah12,m04ah11,m04ah12,m06ah12,m06ah16,m07c0716h10,m07c0716h12,m08ah09,m09ah15,m11ah10,m12ah12,m01b0121h12,m03ah07,m05ah11,m06ah07,m06ah10,m06ah18,m07ah08,m08ah17,m09ah17,m10ah08,m01ah08,m02ah08,m02ah14,m03ah17,m05ah17,m06ah15,m07ah15,m08ah11,m09ah07,m09ah14,m01ah10,m01ah16,m03ah10,m03ah11,m04ah07,m06ah17,m08ah12,m11ah17,m12ah10,m12ah16,m01ah17,m02ah13,m05ah16,m06ah14,m07c0716h11,m09ah11,m09ah18,m10ah09,m10ah13,m11ah16,m12ah15,m01b0121h11,m02ah16,m02ah17,m06ah11,m07ah11,m07ah14,m07c0716h13,m08ah15,m08ah16,m12ah13,m03ah15,m04ah13,m06ah09,m07ah07,m07ah16,m09ah13,m01b0121h13,m03ah14,m04ah09,m04ah15,m06ah08,m07c0716h08,m08ah13,m08ah14,m09ah08,m09ah09,m09ah16,m10ah07,m10ah16,m10ah17,m12ah09,m01b0121h07,m03ah13,m07ah10,m07ah18,m07c0716h14,m08ah08,m08ah10,m11ah14,m12ah08</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2788,7 +2788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B401446D-3BEC-4A29-8153-5548E2976C40}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F36C9C-8F96-49A3-B1AB-C18BB6BBBC79}">
   <dimension ref="B2:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2875,9 +2875,6 @@
       <c r="D7" t="s">
         <v>86</v>
       </c>
-      <c r="E7" t="s">
-        <v>79</v>
-      </c>
       <c r="F7" t="s">
         <v>62</v>
       </c>
@@ -2889,9 +2886,6 @@
       <c r="D8" t="s">
         <v>88</v>
       </c>
-      <c r="E8" t="s">
-        <v>79</v>
-      </c>
       <c r="F8" t="s">
         <v>62</v>
       </c>
@@ -2903,9 +2897,6 @@
       <c r="D9" t="s">
         <v>90</v>
       </c>
-      <c r="E9" t="s">
-        <v>79</v>
-      </c>
       <c r="F9" t="s">
         <v>62</v>
       </c>
@@ -2917,9 +2908,6 @@
       <c r="D10" t="s">
         <v>91</v>
       </c>
-      <c r="E10" t="s">
-        <v>79</v>
-      </c>
       <c r="F10" t="s">
         <v>62</v>
       </c>
@@ -2931,9 +2919,6 @@
       <c r="D11" t="s">
         <v>93</v>
       </c>
-      <c r="E11" t="s">
-        <v>79</v>
-      </c>
       <c r="F11" t="s">
         <v>62</v>
       </c>
@@ -2945,9 +2930,6 @@
       <c r="D12" t="s">
         <v>95</v>
       </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
       <c r="F12" t="s">
         <v>62</v>
       </c>
@@ -2959,9 +2941,6 @@
       <c r="D13" t="s">
         <v>97</v>
       </c>
-      <c r="E13" t="s">
-        <v>79</v>
-      </c>
       <c r="F13" t="s">
         <v>62</v>
       </c>
@@ -2973,9 +2952,6 @@
       <c r="D14" t="s">
         <v>99</v>
       </c>
-      <c r="E14" t="s">
-        <v>79</v>
-      </c>
       <c r="F14" t="s">
         <v>62</v>
       </c>
@@ -2987,9 +2963,6 @@
       <c r="D15" t="s">
         <v>101</v>
       </c>
-      <c r="E15" t="s">
-        <v>79</v>
-      </c>
       <c r="F15" t="s">
         <v>62</v>
       </c>
@@ -2998,9 +2971,6 @@
       <c r="D16" t="s">
         <v>102</v>
       </c>
-      <c r="E16" t="s">
-        <v>79</v>
-      </c>
       <c r="F16" t="s">
         <v>62</v>
       </c>
@@ -3009,9 +2979,6 @@
       <c r="D17" t="s">
         <v>103</v>
       </c>
-      <c r="E17" t="s">
-        <v>79</v>
-      </c>
       <c r="F17" t="s">
         <v>62</v>
       </c>
@@ -3020,9 +2987,6 @@
       <c r="D18" t="s">
         <v>104</v>
       </c>
-      <c r="E18" t="s">
-        <v>79</v>
-      </c>
       <c r="F18" t="s">
         <v>62</v>
       </c>
@@ -3031,9 +2995,6 @@
       <c r="D19" t="s">
         <v>105</v>
       </c>
-      <c r="E19" t="s">
-        <v>79</v>
-      </c>
       <c r="F19" t="s">
         <v>62</v>
       </c>
@@ -3042,9 +3003,6 @@
       <c r="D20" t="s">
         <v>106</v>
       </c>
-      <c r="E20" t="s">
-        <v>79</v>
-      </c>
       <c r="F20" t="s">
         <v>62</v>
       </c>
@@ -3053,9 +3011,6 @@
       <c r="D21" t="s">
         <v>107</v>
       </c>
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
       <c r="F21" t="s">
         <v>62</v>
       </c>
@@ -3064,9 +3019,6 @@
       <c r="D22" t="s">
         <v>108</v>
       </c>
-      <c r="E22" t="s">
-        <v>79</v>
-      </c>
       <c r="F22" t="s">
         <v>62</v>
       </c>
@@ -3075,9 +3027,6 @@
       <c r="D23" t="s">
         <v>109</v>
       </c>
-      <c r="E23" t="s">
-        <v>79</v>
-      </c>
       <c r="F23" t="s">
         <v>62</v>
       </c>
@@ -3086,9 +3035,6 @@
       <c r="D24" t="s">
         <v>110</v>
       </c>
-      <c r="E24" t="s">
-        <v>79</v>
-      </c>
       <c r="F24" t="s">
         <v>62</v>
       </c>
@@ -3097,9 +3043,6 @@
       <c r="D25" t="s">
         <v>111</v>
       </c>
-      <c r="E25" t="s">
-        <v>79</v>
-      </c>
       <c r="F25" t="s">
         <v>62</v>
       </c>
@@ -3108,9 +3051,6 @@
       <c r="D26" t="s">
         <v>112</v>
       </c>
-      <c r="E26" t="s">
-        <v>79</v>
-      </c>
       <c r="F26" t="s">
         <v>62</v>
       </c>
@@ -3119,9 +3059,6 @@
       <c r="D27" t="s">
         <v>113</v>
       </c>
-      <c r="E27" t="s">
-        <v>79</v>
-      </c>
       <c r="F27" t="s">
         <v>62</v>
       </c>
@@ -3130,528 +3067,384 @@
       <c r="D28" t="s">
         <v>114</v>
       </c>
-      <c r="E28" t="s">
-        <v>79</v>
-      </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D29" t="s">
         <v>115</v>
       </c>
-      <c r="E29" t="s">
-        <v>79</v>
-      </c>
       <c r="F29" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D30" t="s">
         <v>116</v>
       </c>
-      <c r="E30" t="s">
-        <v>79</v>
-      </c>
       <c r="F30" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D31" t="s">
         <v>117</v>
       </c>
-      <c r="E31" t="s">
-        <v>79</v>
-      </c>
       <c r="F31" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D32" t="s">
         <v>118</v>
       </c>
-      <c r="E32" t="s">
-        <v>79</v>
-      </c>
       <c r="F32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D33" t="s">
         <v>119</v>
       </c>
-      <c r="E33" t="s">
-        <v>79</v>
-      </c>
       <c r="F33" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D34" t="s">
         <v>120</v>
       </c>
-      <c r="E34" t="s">
-        <v>79</v>
-      </c>
       <c r="F34" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D35" t="s">
         <v>121</v>
       </c>
-      <c r="E35" t="s">
-        <v>79</v>
-      </c>
       <c r="F35" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D36" t="s">
         <v>122</v>
       </c>
-      <c r="E36" t="s">
-        <v>79</v>
-      </c>
       <c r="F36" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D37" t="s">
         <v>123</v>
       </c>
-      <c r="E37" t="s">
-        <v>79</v>
-      </c>
       <c r="F37" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D38" t="s">
         <v>124</v>
       </c>
-      <c r="E38" t="s">
-        <v>79</v>
-      </c>
       <c r="F38" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D39" t="s">
         <v>125</v>
       </c>
-      <c r="E39" t="s">
-        <v>79</v>
-      </c>
       <c r="F39" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D40" t="s">
         <v>126</v>
       </c>
-      <c r="E40" t="s">
-        <v>79</v>
-      </c>
       <c r="F40" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D41" t="s">
         <v>127</v>
       </c>
-      <c r="E41" t="s">
-        <v>79</v>
-      </c>
       <c r="F41" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D42" t="s">
         <v>128</v>
       </c>
-      <c r="E42" t="s">
-        <v>79</v>
-      </c>
       <c r="F42" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D43" t="s">
         <v>129</v>
       </c>
-      <c r="E43" t="s">
-        <v>79</v>
-      </c>
       <c r="F43" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D44" t="s">
         <v>130</v>
       </c>
-      <c r="E44" t="s">
-        <v>79</v>
-      </c>
       <c r="F44" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D45" t="s">
         <v>131</v>
       </c>
-      <c r="E45" t="s">
-        <v>79</v>
-      </c>
       <c r="F45" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D46" t="s">
         <v>132</v>
       </c>
-      <c r="E46" t="s">
-        <v>79</v>
-      </c>
       <c r="F46" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D47" t="s">
         <v>133</v>
       </c>
-      <c r="E47" t="s">
-        <v>79</v>
-      </c>
       <c r="F47" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D48" t="s">
         <v>134</v>
       </c>
-      <c r="E48" t="s">
-        <v>79</v>
-      </c>
       <c r="F48" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D49" t="s">
         <v>135</v>
       </c>
-      <c r="E49" t="s">
-        <v>79</v>
-      </c>
       <c r="F49" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D50" t="s">
         <v>136</v>
       </c>
-      <c r="E50" t="s">
-        <v>79</v>
-      </c>
       <c r="F50" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D51" t="s">
         <v>137</v>
       </c>
-      <c r="E51" t="s">
-        <v>79</v>
-      </c>
       <c r="F51" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D52" t="s">
         <v>138</v>
       </c>
-      <c r="E52" t="s">
-        <v>79</v>
-      </c>
       <c r="F52" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D53" t="s">
         <v>139</v>
       </c>
-      <c r="E53" t="s">
-        <v>79</v>
-      </c>
       <c r="F53" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D54" t="s">
         <v>140</v>
       </c>
-      <c r="E54" t="s">
-        <v>79</v>
-      </c>
       <c r="F54" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D55" t="s">
         <v>141</v>
       </c>
-      <c r="E55" t="s">
-        <v>79</v>
-      </c>
       <c r="F55" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D56" t="s">
         <v>142</v>
       </c>
-      <c r="E56" t="s">
-        <v>79</v>
-      </c>
       <c r="F56" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D57" t="s">
         <v>143</v>
       </c>
-      <c r="E57" t="s">
-        <v>79</v>
-      </c>
       <c r="F57" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D58" t="s">
         <v>144</v>
       </c>
-      <c r="E58" t="s">
-        <v>79</v>
-      </c>
       <c r="F58" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D59" t="s">
         <v>145</v>
       </c>
-      <c r="E59" t="s">
-        <v>79</v>
-      </c>
       <c r="F59" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D60" t="s">
         <v>146</v>
       </c>
-      <c r="E60" t="s">
-        <v>79</v>
-      </c>
       <c r="F60" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D61" t="s">
         <v>147</v>
       </c>
-      <c r="E61" t="s">
-        <v>79</v>
-      </c>
       <c r="F61" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D62" t="s">
         <v>148</v>
       </c>
-      <c r="E62" t="s">
-        <v>79</v>
-      </c>
       <c r="F62" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D63" t="s">
         <v>149</v>
       </c>
-      <c r="E63" t="s">
-        <v>79</v>
-      </c>
       <c r="F63" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D64" t="s">
         <v>150</v>
       </c>
-      <c r="E64" t="s">
-        <v>79</v>
-      </c>
       <c r="F64" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D65" t="s">
         <v>151</v>
       </c>
-      <c r="E65" t="s">
-        <v>79</v>
-      </c>
       <c r="F65" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D66" t="s">
         <v>152</v>
       </c>
-      <c r="E66" t="s">
-        <v>79</v>
-      </c>
       <c r="F66" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D67" t="s">
         <v>153</v>
       </c>
-      <c r="E67" t="s">
-        <v>79</v>
-      </c>
       <c r="F67" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D68" t="s">
         <v>154</v>
       </c>
-      <c r="E68" t="s">
-        <v>79</v>
-      </c>
       <c r="F68" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D69" t="s">
         <v>155</v>
       </c>
-      <c r="E69" t="s">
-        <v>79</v>
-      </c>
       <c r="F69" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D70" t="s">
         <v>156</v>
       </c>
-      <c r="E70" t="s">
-        <v>79</v>
-      </c>
       <c r="F70" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D71" t="s">
         <v>157</v>
       </c>
-      <c r="E71" t="s">
-        <v>79</v>
-      </c>
       <c r="F71" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D72" t="s">
         <v>158</v>
       </c>
-      <c r="E72" t="s">
-        <v>79</v>
-      </c>
       <c r="F72" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D73" t="s">
         <v>159</v>
       </c>
-      <c r="E73" t="s">
-        <v>79</v>
-      </c>
       <c r="F73" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D74" t="s">
         <v>160</v>
       </c>
-      <c r="E74" t="s">
-        <v>79</v>
-      </c>
       <c r="F74" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.45">
       <c r="D75" t="s">
         <v>161</v>
       </c>
-      <c r="E75" t="s">
-        <v>79</v>
-      </c>
       <c r="F75" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3660,7 +3453,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2159FD45-D9B9-4863-A934-13ED648E343B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3074CD41-D92A-4FA0-9544-6625D323A68C}">
   <dimension ref="B2:O339"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3809,10 +3602,10 @@
         <v>168</v>
       </c>
       <c r="M6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="N6">
-        <v>4.5463609172482565E-2</v>
+        <v>5.8624127617148553E-2</v>
       </c>
       <c r="O6" t="s">
         <v>516</v>
@@ -3844,10 +3637,10 @@
         <v>168</v>
       </c>
       <c r="M7" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="N7">
-        <v>0.12203389830508475</v>
+        <v>0.14715852442671987</v>
       </c>
       <c r="O7" t="s">
         <v>516</v>
@@ -3879,10 +3672,10 @@
         <v>168</v>
       </c>
       <c r="M8" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="N8">
-        <v>5.8624127617148553E-2</v>
+        <v>5.0249252243270197E-2</v>
       </c>
       <c r="O8" t="s">
         <v>516</v>
@@ -3914,10 +3707,10 @@
         <v>168</v>
       </c>
       <c r="M9" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="N9">
-        <v>0.1986041874376869</v>
+        <v>7.7766699900299094E-2</v>
       </c>
       <c r="O9" t="s">
         <v>516</v>
@@ -3949,10 +3742,10 @@
         <v>168</v>
       </c>
       <c r="M10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="N10">
-        <v>0.1543369890329013</v>
+        <v>9.2123629112662017E-2</v>
       </c>
       <c r="O10" t="s">
         <v>516</v>
@@ -3984,10 +3777,10 @@
         <v>168</v>
       </c>
       <c r="M11" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="N11">
-        <v>0.16510468594217348</v>
+        <v>4.5463609172482565E-2</v>
       </c>
       <c r="O11" t="s">
         <v>516</v>
@@ -4019,10 +3812,10 @@
         <v>168</v>
       </c>
       <c r="M12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="N12">
-        <v>5.0249252243270197E-2</v>
+        <v>0.12203389830508475</v>
       </c>
       <c r="O12" t="s">
         <v>516</v>
@@ -4054,10 +3847,10 @@
         <v>168</v>
       </c>
       <c r="M13" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="N13">
-        <v>7.7766699900299094E-2</v>
+        <v>0.1986041874376869</v>
       </c>
       <c r="O13" t="s">
         <v>516</v>
@@ -4089,10 +3882,10 @@
         <v>168</v>
       </c>
       <c r="M14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N14">
-        <v>9.2123629112662017E-2</v>
+        <v>0.1543369890329013</v>
       </c>
       <c r="O14" t="s">
         <v>516</v>
@@ -4124,10 +3917,10 @@
         <v>168</v>
       </c>
       <c r="M15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N15">
-        <v>0.14715852442671987</v>
+        <v>0.16510468594217348</v>
       </c>
       <c r="O15" t="s">
         <v>516</v>
@@ -12563,7 +12356,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE042B97-0457-4FD0-9B12-94135A37A91A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121FC73B-6900-424A-BC55-0F37DB294C27}">
   <dimension ref="B2:O647"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>